<commit_message>
informe de caja terminado
</commit_message>
<xml_diff>
--- a/datosTienda.xlsx
+++ b/datosTienda.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f1e0ece63e012e3a/Documentos/UNIVERSIDAD/POO/laboratorio_3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="112" documentId="11_AD4D2F04E46CFB4ACB3E20099597C25A683EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{973A3E7D-428A-40EF-9BB2-A7D2B876F48B}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="11_AD4D2F04E46CFB4ACB3E20099597C25A683EDF1C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C09D8CB3-BD5B-42BF-99FB-738867DFC850}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
   <si>
     <t>id_producto</t>
   </si>
@@ -115,6 +126,18 @@
   </si>
   <si>
     <t>ChiclesZ</t>
+  </si>
+  <si>
+    <t>total:</t>
+  </si>
+  <si>
+    <t>snack:</t>
+  </si>
+  <si>
+    <t>bebida:</t>
+  </si>
+  <si>
+    <t>dulce:</t>
   </si>
 </sst>
 </file>
@@ -150,8 +173,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="149" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="149" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -779,6 +803,88 @@
         <v>25</v>
       </c>
     </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <f>C2*F2</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <f t="shared" ref="C11:C19" si="0">C3*F3</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18">
+        <f>C11+C16</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19">
+        <f>C12+C14</f>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1">
+        <f>(C10+C13+C15)-((C10+C13+C15)*0.2)</f>
+        <v>89.6</v>
+      </c>
+      <c r="D20" s="1">
+        <f>(C10+C13+C15)*0.2</f>
+        <v>22.400000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22">
+        <f>SUM(C18+C19+C20+D20)</f>
+        <v>342</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>